<commit_message>
modified: blinki.py and product sheet file
</commit_message>
<xml_diff>
--- a/product_data.xlsx
+++ b/product_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalit\OneDrive\Desktop\Blinkit Scrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A316B0CF-D3EC-4AC8-909A-84EC2FC68518}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187F2473-746C-44AF-B5FE-B455074E0876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{9B580129-65F9-4172-8259-EC4B60CB8A0B}"/>
   </bookViews>
@@ -836,7 +836,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,487 +858,487 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
+      <c r="A2" s="3">
+        <v>1840767</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
+        <v>1853552</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>1337069</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>1165686</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>1092739</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>1518161</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>1840729</v>
+        <v>1092739</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>1705981</v>
+        <v>1518161</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>1857338</v>
+        <v>1840729</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>1857345</v>
+        <v>1705981</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>21192</v>
+        <v>1857338</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>58760</v>
+        <v>1857345</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>1840682</v>
+        <v>21192</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>4759</v>
+        <v>58760</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>21493</v>
+        <v>1840682</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>41</v>
+      <c r="A19" s="3">
+        <v>4759</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>1792288</v>
+        <v>21493</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>1296434</v>
+        <v>1792288</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>1518277</v>
+        <v>1296434</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>1842389</v>
+      <c r="A25" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>1434768</v>
+        <v>1518277</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>60</v>
+      <c r="A27" s="3">
+        <v>1842389</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>1840767</v>
+        <v>1434768</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>1480123</v>
+      <c r="A29" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>1842396</v>
+        <v>1480123</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>4755</v>
+        <v>1842396</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
+        <v>4755</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>1518260</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>21198</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>4753</v>
+        <v>21198</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>21495</v>
+        <v>4753</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>1518130</v>
+        <v>21495</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>1705998</v>
+        <v>1518130</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>1661638</v>
+        <v>1705998</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>4080</v>
+        <v>1661638</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>21102</v>
+        <v>4080</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
+        <v>21102</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>1480147</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>1840828</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>1853552</v>
+        <v>1840828</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,61 +1464,60 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A0314937-EBE4-4690-9ECD-0D233F9867D5}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{1B73BA47-DCE7-42F6-A4B9-722B3AEE120A}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{37FB4136-3581-4EE7-BFA9-7870BDC930C0}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{7827C92C-E3FA-4AC1-8263-B2C43CF1A5E1}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{7338A8A7-E8D1-45A8-8C0A-5369FE53E6A8}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{997B8099-CB1F-444B-917C-0653107812DC}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{1E0CDBBD-E22C-42EC-83C2-F555D11A7226}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{DDFF3E30-3B96-4BAB-A35D-A516E933BB8C}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{B0E3A297-BDD8-4FB1-9288-F6D4688FB80E}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{1EBC7EFB-1FF1-4C7C-AC61-F151F5CF6BA5}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{7D9A7AB9-43FE-4FEF-B5A3-2D98CB9C40A7}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{D6605325-784C-46E0-86AC-519ED1D66230}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{A9362E34-D045-465D-8A08-6C8D0A573672}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{ED051E19-59EB-449D-B4D6-EDCFBD66B2CA}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{0996A338-3318-4014-8D86-5B2778972880}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{4C600012-4975-4D9F-8BF5-A5A022CDCCAF}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{33959C2B-20D6-4F50-94D9-AE93E68E64A6}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{F986842E-0345-42C0-AA6A-CBAA906D103A}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{1F60D4E6-D51A-4286-BEC2-88B46C173DE3}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{9C74141F-5E01-478A-9000-DD1E53DE0DC0}"/>
-    <hyperlink ref="C22" r:id="rId21" xr:uid="{3B253E42-61B1-4632-A8BB-BDA475459BAE}"/>
-    <hyperlink ref="C23" r:id="rId22" xr:uid="{47028FAB-2B63-45D2-97A8-49492A87B28A}"/>
-    <hyperlink ref="C24" r:id="rId23" xr:uid="{C7F987DA-0C98-4FE6-BFA5-62C003942C99}"/>
-    <hyperlink ref="C25" r:id="rId24" xr:uid="{995BDA0E-F14E-4827-8A5B-2952E0361DC5}"/>
-    <hyperlink ref="C26" r:id="rId25" xr:uid="{0DFB7959-F1B3-4C37-B897-5CA65B11FF5B}"/>
-    <hyperlink ref="C27" r:id="rId26" xr:uid="{DDAF3813-389E-4BB9-9066-5C4ABD340085}"/>
-    <hyperlink ref="C28" r:id="rId27" xr:uid="{29FF52B3-B95C-465C-8AC4-845CA84B3C78}"/>
-    <hyperlink ref="C29" r:id="rId28" xr:uid="{28366DAF-6335-47F0-9860-1DBC7B1186D8}"/>
-    <hyperlink ref="C30" r:id="rId29" xr:uid="{0FB3D5A4-D7BE-4C2D-AF1E-504DDA473713}"/>
-    <hyperlink ref="C31" r:id="rId30" xr:uid="{D72C7531-3D29-4599-B110-C543E15ACA23}"/>
-    <hyperlink ref="C32" r:id="rId31" xr:uid="{4FA6C0A7-3804-4514-BCDC-71BFF16B8943}"/>
-    <hyperlink ref="C33" r:id="rId32" xr:uid="{15D232C8-1CFD-45C0-BA30-53E2E1414C4F}"/>
-    <hyperlink ref="C34" r:id="rId33" xr:uid="{F9B38C9E-9BCA-4202-919B-7BF1074E8D19}"/>
-    <hyperlink ref="C35" r:id="rId34" xr:uid="{C4761837-0C2E-42E6-8536-5CB03417A1FC}"/>
-    <hyperlink ref="C36" r:id="rId35" xr:uid="{B9ED7F2F-2309-483A-974A-C15894F80C16}"/>
-    <hyperlink ref="C37" r:id="rId36" xr:uid="{46EC4D08-1D4B-427C-977E-99183EF5D0A4}"/>
-    <hyperlink ref="C38" r:id="rId37" xr:uid="{AC91C471-5E96-45A5-900E-019C3C39800F}"/>
-    <hyperlink ref="C39" r:id="rId38" xr:uid="{8ECF5ADA-E533-4EBA-859D-ED72A33BB6B8}"/>
-    <hyperlink ref="C40" r:id="rId39" xr:uid="{D0270CB1-96A3-4D69-B73B-DD687C3A74C0}"/>
-    <hyperlink ref="C41" r:id="rId40" xr:uid="{C8920017-B1E9-46CC-93DD-F160D3E0624B}"/>
-    <hyperlink ref="C42" r:id="rId41" xr:uid="{22F96188-6ADA-4A54-A770-BFF0EA7575CA}"/>
-    <hyperlink ref="C43" r:id="rId42" xr:uid="{C6B589DF-E6A2-4D7E-9F44-C399E02E9900}"/>
-    <hyperlink ref="C44" r:id="rId43" xr:uid="{33EE0296-8A04-4D90-8F36-1177AF960B96}"/>
-    <hyperlink ref="C45" r:id="rId44" xr:uid="{D4B6C588-99FA-4185-BCC6-BCD8D8BB6955}"/>
-    <hyperlink ref="C46" r:id="rId45" xr:uid="{58ADF1E8-366E-4B2B-835A-A65BA70A3864}"/>
-    <hyperlink ref="C47" r:id="rId46" xr:uid="{150E43B3-851D-4E88-87B0-25115BFD8C4D}"/>
-    <hyperlink ref="C48" r:id="rId47" xr:uid="{7C473C12-1A30-4FA8-94EE-DD410857905F}"/>
-    <hyperlink ref="C49" r:id="rId48" xr:uid="{4F0CA22D-FD01-42B3-A91B-DBDBB408D4D5}"/>
-    <hyperlink ref="C50" r:id="rId49" xr:uid="{E58B3C7F-B462-407D-B8BC-74D0EF55CD5E}"/>
-    <hyperlink ref="C51" r:id="rId50" xr:uid="{929FCD43-9DEB-4EC5-9DE4-21C6B0E196D7}"/>
-    <hyperlink ref="C52" r:id="rId51" xr:uid="{87758105-63ED-42DA-843D-AE48DC8A54AB}"/>
-    <hyperlink ref="C53" r:id="rId52" xr:uid="{CD7E236B-DCF5-4A74-950E-09B0421B7643}"/>
-    <hyperlink ref="C54" r:id="rId53" xr:uid="{2D3A8FD8-5075-4ACE-9B13-370EE6E33846}"/>
-    <hyperlink ref="C55" r:id="rId54" xr:uid="{226B1E4E-661C-4FD3-B352-8371CB3F4301}"/>
-    <hyperlink ref="C56" r:id="rId55" xr:uid="{669E2DF0-0553-419A-A5EC-F895F3277949}"/>
+    <hyperlink ref="C8" r:id="rId1" xr:uid="{7338A8A7-E8D1-45A8-8C0A-5369FE53E6A8}"/>
+    <hyperlink ref="C9" r:id="rId2" xr:uid="{997B8099-CB1F-444B-917C-0653107812DC}"/>
+    <hyperlink ref="C10" r:id="rId3" xr:uid="{1E0CDBBD-E22C-42EC-83C2-F555D11A7226}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{DDFF3E30-3B96-4BAB-A35D-A516E933BB8C}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{B0E3A297-BDD8-4FB1-9288-F6D4688FB80E}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{1EBC7EFB-1FF1-4C7C-AC61-F151F5CF6BA5}"/>
+    <hyperlink ref="C14" r:id="rId7" xr:uid="{7D9A7AB9-43FE-4FEF-B5A3-2D98CB9C40A7}"/>
+    <hyperlink ref="C15" r:id="rId8" xr:uid="{D6605325-784C-46E0-86AC-519ED1D66230}"/>
+    <hyperlink ref="C16" r:id="rId9" xr:uid="{A9362E34-D045-465D-8A08-6C8D0A573672}"/>
+    <hyperlink ref="C17" r:id="rId10" xr:uid="{ED051E19-59EB-449D-B4D6-EDCFBD66B2CA}"/>
+    <hyperlink ref="C18" r:id="rId11" xr:uid="{0996A338-3318-4014-8D86-5B2778972880}"/>
+    <hyperlink ref="C19" r:id="rId12" xr:uid="{4C600012-4975-4D9F-8BF5-A5A022CDCCAF}"/>
+    <hyperlink ref="C20" r:id="rId13" xr:uid="{33959C2B-20D6-4F50-94D9-AE93E68E64A6}"/>
+    <hyperlink ref="C21" r:id="rId14" xr:uid="{F986842E-0345-42C0-AA6A-CBAA906D103A}"/>
+    <hyperlink ref="C22" r:id="rId15" xr:uid="{1F60D4E6-D51A-4286-BEC2-88B46C173DE3}"/>
+    <hyperlink ref="C23" r:id="rId16" xr:uid="{9C74141F-5E01-478A-9000-DD1E53DE0DC0}"/>
+    <hyperlink ref="C24" r:id="rId17" xr:uid="{3B253E42-61B1-4632-A8BB-BDA475459BAE}"/>
+    <hyperlink ref="C25" r:id="rId18" xr:uid="{47028FAB-2B63-45D2-97A8-49492A87B28A}"/>
+    <hyperlink ref="C26" r:id="rId19" xr:uid="{C7F987DA-0C98-4FE6-BFA5-62C003942C99}"/>
+    <hyperlink ref="C27" r:id="rId20" xr:uid="{995BDA0E-F14E-4827-8A5B-2952E0361DC5}"/>
+    <hyperlink ref="C28" r:id="rId21" xr:uid="{0DFB7959-F1B3-4C37-B897-5CA65B11FF5B}"/>
+    <hyperlink ref="C29" r:id="rId22" xr:uid="{DDAF3813-389E-4BB9-9066-5C4ABD340085}"/>
+    <hyperlink ref="C2" r:id="rId23" xr:uid="{29FF52B3-B95C-465C-8AC4-845CA84B3C78}"/>
+    <hyperlink ref="C30" r:id="rId24" xr:uid="{28366DAF-6335-47F0-9860-1DBC7B1186D8}"/>
+    <hyperlink ref="C31" r:id="rId25" xr:uid="{0FB3D5A4-D7BE-4C2D-AF1E-504DDA473713}"/>
+    <hyperlink ref="C32" r:id="rId26" xr:uid="{D72C7531-3D29-4599-B110-C543E15ACA23}"/>
+    <hyperlink ref="C33" r:id="rId27" xr:uid="{4FA6C0A7-3804-4514-BCDC-71BFF16B8943}"/>
+    <hyperlink ref="C34" r:id="rId28" xr:uid="{15D232C8-1CFD-45C0-BA30-53E2E1414C4F}"/>
+    <hyperlink ref="C35" r:id="rId29" xr:uid="{F9B38C9E-9BCA-4202-919B-7BF1074E8D19}"/>
+    <hyperlink ref="C36" r:id="rId30" xr:uid="{C4761837-0C2E-42E6-8536-5CB03417A1FC}"/>
+    <hyperlink ref="C37" r:id="rId31" xr:uid="{B9ED7F2F-2309-483A-974A-C15894F80C16}"/>
+    <hyperlink ref="C38" r:id="rId32" xr:uid="{46EC4D08-1D4B-427C-977E-99183EF5D0A4}"/>
+    <hyperlink ref="C39" r:id="rId33" xr:uid="{AC91C471-5E96-45A5-900E-019C3C39800F}"/>
+    <hyperlink ref="C40" r:id="rId34" xr:uid="{8ECF5ADA-E533-4EBA-859D-ED72A33BB6B8}"/>
+    <hyperlink ref="C41" r:id="rId35" xr:uid="{D0270CB1-96A3-4D69-B73B-DD687C3A74C0}"/>
+    <hyperlink ref="C42" r:id="rId36" xr:uid="{C8920017-B1E9-46CC-93DD-F160D3E0624B}"/>
+    <hyperlink ref="C43" r:id="rId37" xr:uid="{22F96188-6ADA-4A54-A770-BFF0EA7575CA}"/>
+    <hyperlink ref="C44" r:id="rId38" xr:uid="{C6B589DF-E6A2-4D7E-9F44-C399E02E9900}"/>
+    <hyperlink ref="C45" r:id="rId39" xr:uid="{33EE0296-8A04-4D90-8F36-1177AF960B96}"/>
+    <hyperlink ref="C3" r:id="rId40" display="https://blinkit.com/prn/m/prid/504593/" xr:uid="{D4B6C588-99FA-4185-BCC6-BCD8D8BB6955}"/>
+    <hyperlink ref="C46" r:id="rId41" xr:uid="{58ADF1E8-366E-4B2B-835A-A65BA70A3864}"/>
+    <hyperlink ref="C47" r:id="rId42" xr:uid="{150E43B3-851D-4E88-87B0-25115BFD8C4D}"/>
+    <hyperlink ref="C48" r:id="rId43" xr:uid="{7C473C12-1A30-4FA8-94EE-DD410857905F}"/>
+    <hyperlink ref="C49" r:id="rId44" xr:uid="{4F0CA22D-FD01-42B3-A91B-DBDBB408D4D5}"/>
+    <hyperlink ref="C50" r:id="rId45" xr:uid="{E58B3C7F-B462-407D-B8BC-74D0EF55CD5E}"/>
+    <hyperlink ref="C51" r:id="rId46" xr:uid="{929FCD43-9DEB-4EC5-9DE4-21C6B0E196D7}"/>
+    <hyperlink ref="C52" r:id="rId47" xr:uid="{87758105-63ED-42DA-843D-AE48DC8A54AB}"/>
+    <hyperlink ref="C53" r:id="rId48" xr:uid="{CD7E236B-DCF5-4A74-950E-09B0421B7643}"/>
+    <hyperlink ref="C54" r:id="rId49" xr:uid="{2D3A8FD8-5075-4ACE-9B13-370EE6E33846}"/>
+    <hyperlink ref="C55" r:id="rId50" xr:uid="{226B1E4E-661C-4FD3-B352-8371CB3F4301}"/>
+    <hyperlink ref="C56" r:id="rId51" xr:uid="{669E2DF0-0553-419A-A5EC-F895F3277949}"/>
+    <hyperlink ref="C7" r:id="rId52" xr:uid="{7827C92C-E3FA-4AC1-8263-B2C43CF1A5E1}"/>
+    <hyperlink ref="C6" r:id="rId53" xr:uid="{37FB4136-3581-4EE7-BFA9-7870BDC930C0}"/>
+    <hyperlink ref="C5" r:id="rId54" xr:uid="{1B73BA47-DCE7-42F6-A4B9-722B3AEE120A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
code optmisation and enabled multi pincode search
</commit_message>
<xml_diff>
--- a/product_data.xlsx
+++ b/product_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lalit\OneDrive\Desktop\Blinkit Scrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187F2473-746C-44AF-B5FE-B455074E0876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694BC36A-FDD2-4F0B-BA81-611859863C19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{9B580129-65F9-4172-8259-EC4B60CB8A0B}"/>
   </bookViews>
@@ -27,15 +27,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
-    <t>Sku Code</t>
-  </si>
-  <si>
     <t>Product Name</t>
   </si>
   <si>
-    <t>Blinkit</t>
-  </si>
-  <si>
     <t>GC990</t>
   </si>
   <si>
@@ -406,6 +400,12 @@
   </si>
   <si>
     <t>https://blinkit.com/prn/m/prid/625472/</t>
+  </si>
+  <si>
+    <t>Product Url</t>
+  </si>
+  <si>
+    <t>SKU Code</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,13 +848,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,10 +862,10 @@
         <v>1840767</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -873,21 +873,21 @@
         <v>1853552</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,10 +895,10 @@
         <v>1337069</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,43 +906,43 @@
         <v>1165686</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,10 +950,10 @@
         <v>1092739</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,10 +961,10 @@
         <v>1518161</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,10 +972,10 @@
         <v>1840729</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -983,10 +983,10 @@
         <v>1705981</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -994,10 +994,10 @@
         <v>1857338</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,10 +1005,10 @@
         <v>1857345</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,10 +1016,10 @@
         <v>21192</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,10 +1027,10 @@
         <v>58760</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1038,10 +1038,10 @@
         <v>1840682</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1049,10 +1049,10 @@
         <v>4759</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,21 +1060,21 @@
         <v>21493</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,21 +1082,21 @@
         <v>1792288</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1104,21 +1104,21 @@
         <v>1296434</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1126,10 +1126,10 @@
         <v>1518277</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,10 +1137,10 @@
         <v>1842389</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1148,21 +1148,21 @@
         <v>1434768</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,10 +1170,10 @@
         <v>1480123</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>1842396</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1192,10 +1192,10 @@
         <v>4755</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1203,21 +1203,21 @@
         <v>1518260</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1225,10 +1225,10 @@
         <v>21198</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1236,10 +1236,10 @@
         <v>4753</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,10 +1247,10 @@
         <v>21495</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1258,10 +1258,10 @@
         <v>1518130</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1269,10 +1269,10 @@
         <v>1705998</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1280,10 +1280,10 @@
         <v>1661638</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,10 +1291,10 @@
         <v>4080</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1302,10 +1302,10 @@
         <v>21102</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1313,21 +1313,21 @@
         <v>1480147</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1335,10 +1335,10 @@
         <v>1840828</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1346,21 +1346,21 @@
         <v>1843621</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1368,10 +1368,10 @@
         <v>1157674</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1379,21 +1379,21 @@
         <v>1480154</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1401,21 +1401,21 @@
         <v>1479660</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1423,21 +1423,21 @@
         <v>1843638</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1445,10 +1445,10 @@
         <v>1853521</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1456,10 +1456,10 @@
         <v>1823609</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>